<commit_message>
Update in registration test
</commit_message>
<xml_diff>
--- a/com.DemowebShop/src/main/resources/DataDocuments/TestData.xlsx
+++ b/com.DemowebShop/src/main/resources/DataDocuments/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUGANDHA GOEL\LearningAutomation\com.DemowebShop\src\main\resources\DataDocuments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUGANDHA GOEL\git\QSpiderDemoWebShopProject\com.DemowebShop\src\main\resources\DataDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18480A77-FF6A-41A9-9DC8-90C68F5A79B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5E53E0-3790-4B4C-B626-516C17DEBB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Gender</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>yjensen@gmail.com</t>
-  </si>
-  <si>
     <t>%q*cJE8Zo7</t>
   </si>
   <si>
@@ -127,10 +124,16 @@
     <t>Agarwal</t>
   </si>
   <si>
-    <t>akhil@gmail.com</t>
-  </si>
-  <si>
     <t>1234567!</t>
+  </si>
+  <si>
+    <t>yjensen8482418@gmail.com</t>
+  </si>
+  <si>
+    <t>bethany65@gmail.com</t>
+  </si>
+  <si>
+    <t>akhilagarwal012@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -198,12 +201,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -488,12 +492,13 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -523,52 +528,53 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
         <v>32</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{CA693283-30A4-4B4B-90FA-9B4C27AC0F54}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{B3E9FED0-3C23-4ECD-869D-EE2042FA3979}"/>
-    <hyperlink ref="E4" r:id="rId3" display="1234567@" xr:uid="{AC0D4552-04FC-4703-8D88-C0FA89FBF821}"/>
+    <hyperlink ref="E4" r:id="rId1" display="1234567@" xr:uid="{AC0D4552-04FC-4703-8D88-C0FA89FBF821}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{D6DA466D-9550-4391-85A1-6CED8250B9FB}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{8934DA79-BCBC-45D2-97EE-7535C9129B6A}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{46973C1A-0026-41A7-857B-31280EEBA5F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -590,74 +596,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
         <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Listner added in repo
</commit_message>
<xml_diff>
--- a/com.DemowebShop/src/main/resources/DataDocuments/TestData.xlsx
+++ b/com.DemowebShop/src/main/resources/DataDocuments/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUGANDHA GOEL\git\QSpiderDemoWebShopProject\com.DemowebShop\src\main\resources\DataDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5E53E0-3790-4B4C-B626-516C17DEBB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4BD558-47C5-4986-994D-926958313781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Gender</t>
   </si>
@@ -37,9 +37,6 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -125,15 +122,6 @@
   </si>
   <si>
     <t>1234567!</t>
-  </si>
-  <si>
-    <t>yjensen8482418@gmail.com</t>
-  </si>
-  <si>
-    <t>bethany65@gmail.com</t>
-  </si>
-  <si>
-    <t>akhilagarwal012@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -201,13 +189,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -489,19 +476,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="39.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,67 +500,52 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" display="1234567@" xr:uid="{AC0D4552-04FC-4703-8D88-C0FA89FBF821}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{D6DA466D-9550-4391-85A1-6CED8250B9FB}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{8934DA79-BCBC-45D2-97EE-7535C9129B6A}"/>
-    <hyperlink ref="D2" r:id="rId4" xr:uid="{46973C1A-0026-41A7-857B-31280EEBA5F6}"/>
+    <hyperlink ref="D4" r:id="rId1" display="1234567@" xr:uid="{AC0D4552-04FC-4703-8D88-C0FA89FBF821}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -596,74 +567,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>